<commit_message>
swap SE3A SE3B eic. Add NO2A-NL+NO2A-DE lineset
</commit_message>
<xml_diff>
--- a/data/topology_ig107.xlsx
+++ b/data/topology_ig107.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordicrsc-my.sharepoint.com/personal/jlm_nordic-rcc_net/Documents/Dokumenter/topology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="597" documentId="8_{28EFB05D-36F0-44BB-AB8B-754CA84D9619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C62F0B1-F222-4116-8244-A6A165B5EDF7}"/>
+  <xr:revisionPtr revIDLastSave="643" documentId="8_{28EFB05D-36F0-44BB-AB8B-754CA84D9619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AB9E6CD-C24E-41E9-A7FA-C5E4E593EEFF}"/>
   <bookViews>
-    <workbookView xWindow="44295" yWindow="2010" windowWidth="14340" windowHeight="7245" xr2:uid="{4FBD8BC6-F0E3-4971-A871-8AE8F24F6C5A}"/>
+    <workbookView xWindow="28680" yWindow="-5490" windowWidth="38640" windowHeight="21120" xr2:uid="{4FBD8BC6-F0E3-4971-A871-8AE8F24F6C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="metaData" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="227">
   <si>
     <t>DK1</t>
   </si>
@@ -690,13 +690,37 @@
     <t>topology_ig107</t>
   </si>
   <si>
-    <t>2024-08-12</t>
-  </si>
-  <si>
     <t>topologyType</t>
   </si>
   <si>
-    <t>ntcMarket</t>
+    <t>NtcMarket</t>
+  </si>
+  <si>
+    <t>NO2_ND-NO2A</t>
+  </si>
+  <si>
+    <t>NO2_NK-NO2A</t>
+  </si>
+  <si>
+    <t>["NO2_ND-NO2"]</t>
+  </si>
+  <si>
+    <t>["NO2_NK-NO2"]</t>
+  </si>
+  <si>
+    <t>NO2A-NO2_ND</t>
+  </si>
+  <si>
+    <t>NO2A-NO2_NK</t>
+  </si>
+  <si>
+    <t>["NO2-NO2_ND"]</t>
+  </si>
+  <si>
+    <t>["NO2-NO2_NK"]</t>
+  </si>
+  <si>
+    <t>2-07-2025</t>
   </si>
 </sst>
 </file>
@@ -816,10 +840,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{381C518C-F7D3-4D01-B7CD-B5D6164BCA72}" name="Table1" displayName="Table1" ref="A1:D1048561" totalsRowShown="0">
-  <autoFilter ref="A1:D1048561" xr:uid="{381C518C-F7D3-4D01-B7CD-B5D6164BCA72}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D85">
-    <sortCondition ref="A1:A1048561"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{381C518C-F7D3-4D01-B7CD-B5D6164BCA72}" name="Table1" displayName="Table1" ref="A1:D1048565" totalsRowShown="0">
+  <autoFilter ref="A1:D1048565" xr:uid="{381C518C-F7D3-4D01-B7CD-B5D6164BCA72}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D89">
+    <sortCondition ref="A1:A1048565"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{45520633-A776-43BF-907C-2FF48DC85F39}" name="name"/>
@@ -1154,7 +1178,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1179,7 +1203,7 @@
         <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1187,16 +1211,16 @@
         <v>215</v>
       </c>
       <c r="B2" s="3">
-        <v>1.1000000000000001</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1212,7 +1236,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1667,7 +1691,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -1684,7 +1708,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>184</v>
@@ -1812,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6106AD-B8E1-4460-AC6F-62DB62A8D837}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A85"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2288,27 +2312,27 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>219</v>
       </c>
       <c r="B35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" t="s">
         <v>37</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
       </c>
       <c r="D35" t="s">
         <v>47</v>
@@ -2316,27 +2340,27 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>199</v>
       </c>
       <c r="B36" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="C36" t="s">
-        <v>0</v>
-      </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
         <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>181</v>
       </c>
       <c r="D37" t="s">
         <v>47</v>
@@ -2344,55 +2368,55 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="D39" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D41" t="s">
         <v>45</v>
@@ -2400,83 +2424,83 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>222</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
       <c r="D43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>223</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>171</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D47" t="s">
         <v>50</v>
@@ -2484,13 +2508,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -2498,13 +2522,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
         <v>14</v>
-      </c>
-      <c r="C49" t="s">
-        <v>12</v>
       </c>
       <c r="D49" t="s">
         <v>50</v>
@@ -2512,13 +2536,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
         <v>50</v>
@@ -2526,10 +2550,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
@@ -2540,13 +2564,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>172</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
         <v>50</v>
@@ -2554,13 +2578,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D53" t="s">
         <v>50</v>
@@ -2568,13 +2592,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D54" t="s">
         <v>50</v>
@@ -2582,13 +2606,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
         <v>50</v>
@@ -2596,13 +2620,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
         <v>50</v>
@@ -2610,13 +2634,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D57" t="s">
         <v>50</v>
@@ -2624,10 +2648,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C58" t="s">
         <v>12</v>
@@ -2638,13 +2662,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
         <v>50</v>
@@ -2652,13 +2676,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D60" t="s">
         <v>50</v>
@@ -2666,13 +2690,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
         <v>20</v>
-      </c>
-      <c r="C61" t="s">
-        <v>22</v>
       </c>
       <c r="D61" t="s">
         <v>50</v>
@@ -2680,69 +2704,69 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>208</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="C63" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D63" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="C64" t="s">
-        <v>133</v>
+        <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>181</v>
+        <v>22</v>
       </c>
       <c r="D65" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D66" t="s">
         <v>47</v>
@@ -2750,41 +2774,41 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>173</v>
+        <v>208</v>
       </c>
       <c r="B67" t="s">
-        <v>26</v>
+        <v>209</v>
       </c>
       <c r="C67" t="s">
-        <v>182</v>
+        <v>22</v>
       </c>
       <c r="D67" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="D68" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>187</v>
+        <v>92</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C69" t="s">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="D69" t="s">
         <v>47</v>
@@ -2792,13 +2816,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B70" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C70" t="s">
-        <v>181</v>
+        <v>8</v>
       </c>
       <c r="D70" t="s">
         <v>47</v>
@@ -2806,111 +2830,111 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>182</v>
       </c>
       <c r="D71" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="C72" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D72" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>187</v>
       </c>
       <c r="B73" t="s">
         <v>22</v>
       </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>207</v>
+        <v>79</v>
       </c>
       <c r="B74" t="s">
         <v>22</v>
       </c>
       <c r="C74" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="D74" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B75" t="s">
         <v>22</v>
       </c>
       <c r="C75" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B76" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C76" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D76" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>175</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
       <c r="C77" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D77" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>22</v>
       </c>
       <c r="C78" t="s">
-        <v>24</v>
+        <v>209</v>
       </c>
       <c r="D78" t="s">
         <v>45</v>
@@ -2918,69 +2942,69 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>177</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="C79" t="s">
         <v>24</v>
       </c>
       <c r="D79" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>133</v>
+        <v>30</v>
       </c>
       <c r="C80" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="D80" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
       <c r="B81" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" t="s">
         <v>24</v>
       </c>
-      <c r="C81" t="s">
-        <v>4</v>
-      </c>
       <c r="D81" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="B82" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" t="s">
         <v>24</v>
       </c>
-      <c r="C82" t="s">
-        <v>22</v>
-      </c>
       <c r="D82" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B83" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" t="s">
         <v>24</v>
-      </c>
-      <c r="C83" t="s">
-        <v>152</v>
       </c>
       <c r="D83" t="s">
         <v>45</v>
@@ -2988,13 +3012,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>179</v>
+        <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>24</v>
+        <v>133</v>
       </c>
       <c r="C84" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="D84" t="s">
         <v>45</v>
@@ -3002,15 +3026,71 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>180</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
         <v>24</v>
       </c>
       <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" t="s">
+        <v>22</v>
+      </c>
+      <c r="D86" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>178</v>
+      </c>
+      <c r="B87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" t="s">
+        <v>152</v>
+      </c>
+      <c r="D87" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" t="s">
+        <v>154</v>
+      </c>
+      <c r="D88" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" t="s">
         <v>137</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D89" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3206,10 +3286,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB1DB88-C101-4427-8092-C8804A19573F}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3386,7 +3466,40 @@
         <v>205</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" t="s">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
swapped SE3A and B EICs yet again...
</commit_message>
<xml_diff>
--- a/data/topology_ig107.xlsx
+++ b/data/topology_ig107.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordicrsc-my.sharepoint.com/personal/jlm_nordic-rcc_net/Documents/Dokumenter/topology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="643" documentId="8_{28EFB05D-36F0-44BB-AB8B-754CA84D9619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AB9E6CD-C24E-41E9-A7FA-C5E4E593EEFF}"/>
+  <xr:revisionPtr revIDLastSave="648" documentId="8_{28EFB05D-36F0-44BB-AB8B-754CA84D9619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6075E8B8-69A1-40B4-A464-DC94FAC1F3B1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5490" windowWidth="38640" windowHeight="21120" xr2:uid="{4FBD8BC6-F0E3-4971-A871-8AE8F24F6C5A}"/>
+    <workbookView xWindow="38280" yWindow="15" windowWidth="38640" windowHeight="21120" xr2:uid="{4FBD8BC6-F0E3-4971-A871-8AE8F24F6C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="metaData" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="226">
   <si>
     <t>DK1</t>
   </si>
@@ -718,17 +718,15 @@
   </si>
   <si>
     <t>["NO2-NO2_NK"]</t>
-  </si>
-  <si>
-    <t>2-07-2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -787,12 +785,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1184,8 +1183,8 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1193,10 +1192,10 @@
       <c r="A1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>214</v>
       </c>
       <c r="D1" t="s">
@@ -1210,11 +1209,11 @@
       <c r="A2" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="3">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>226</v>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45707</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
@@ -1228,6 +1227,7 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D849FDEE-CCBB-4171-90DA-0AFD6AD68A79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1236,7 +1236,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
         <v>184</v>
@@ -3382,7 +3382,7 @@
       <c r="A11" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>